<commit_message>
support multiple biosample IDs for trackhubs submission
</commit_message>
<xml_diff>
--- a/src/assets/with_examples/trackhubs.xlsx
+++ b/src/assets/with_examples/trackhubs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hub Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -39,19 +39,19 @@
     <t xml:space="preserve">Description File Path</t>
   </si>
   <si>
-    <t xml:space="preserve">test_hub</t>
+    <t xml:space="preserve">Test Hub</t>
   </si>
   <si>
     <t xml:space="preserve">test</t>
   </si>
   <si>
-    <t xml:space="preserve">test hub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test@ebi.ac.uk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testing trackhubs</t>
+    <t xml:space="preserve">Hub with test data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test@someplace.ac.uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_hub.html</t>
   </si>
   <si>
     <t xml:space="preserve">Assembly Accession</t>
@@ -66,7 +66,10 @@
     <t xml:space="preserve">GCA_000003025.6</t>
   </si>
   <si>
-    <t xml:space="preserve">test_organism</t>
+    <t xml:space="preserve">Pig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pig Genome</t>
   </si>
   <si>
     <t xml:space="preserve">Track Name</t>
@@ -84,10 +87,10 @@
     <t xml:space="preserve">Subdirectory</t>
   </si>
   <si>
-    <t xml:space="preserve">track1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test-hub/test4.Bigbed</t>
+    <t xml:space="preserve">Track1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test-hub/test1.Bigbed</t>
   </si>
   <si>
     <t xml:space="preserve">bigBed</t>
@@ -96,28 +99,74 @@
     <t xml:space="preserve">t1</t>
   </si>
   <si>
-    <t xml:space="preserve">test 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMEA104728909</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">track2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test-hub/test2.Bigbed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test2</t>
+    <t xml:space="preserve">test track 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SAMEA104728908, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">SAMEA104728909</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_dir1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Track2_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test-hub/test2_1.Bigbed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test track 2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMEA104728909, SAMEA104728910</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_dir2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Track2_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test-hub/test2_2.Bigbed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test track 2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMEA104728907</t>
   </si>
 </sst>
 </file>
@@ -127,7 +176,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -172,6 +221,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -216,7 +271,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -229,8 +284,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -257,11 +320,13 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.12"/>
   </cols>
   <sheetData>
@@ -282,7 +347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -300,6 +365,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="test@someplace.ac.uk"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -317,13 +385,14 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -346,7 +415,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -365,85 +434,111 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="24.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="3" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="20.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="3" width="12.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="F2" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="0" t="s">
+      <c r="E3" s="6" t="s">
         <v>31</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update trackhubs example file
</commit_message>
<xml_diff>
--- a/src/assets/with_examples/trackhubs.xlsx
+++ b/src/assets/with_examples/trackhubs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hub Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -39,7 +39,7 @@
     <t xml:space="preserve">Description File Path</t>
   </si>
   <si>
-    <t xml:space="preserve">Test Hub</t>
+    <t xml:space="preserve">Test_Hub</t>
   </si>
   <si>
     <t xml:space="preserve">test</t>
@@ -90,7 +90,7 @@
     <t xml:space="preserve">Track1</t>
   </si>
   <si>
-    <t xml:space="preserve">test-hub/test1.Bigbed</t>
+    <t xml:space="preserve">test1.Bigbed</t>
   </si>
   <si>
     <t xml:space="preserve">bigBed</t>
@@ -102,35 +102,7 @@
     <t xml:space="preserve">test track 1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">SAMEA104728908, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">SAMEA104728909</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t xml:space="preserve">SAMEA104728908, SAMEA104728909 </t>
   </si>
   <si>
     <t xml:space="preserve">sub_dir1</t>
@@ -139,7 +111,7 @@
     <t xml:space="preserve">Track2_1</t>
   </si>
   <si>
-    <t xml:space="preserve">test-hub/test2_1.Bigbed</t>
+    <t xml:space="preserve">test2.Bigbed</t>
   </si>
   <si>
     <t xml:space="preserve">t2.1</t>
@@ -148,7 +120,7 @@
     <t xml:space="preserve">test track 2.1</t>
   </si>
   <si>
-    <t xml:space="preserve">SAMEA104728909, SAMEA104728910</t>
+    <t xml:space="preserve">SAMEA104728909, SAMEA104728907</t>
   </si>
   <si>
     <t xml:space="preserve">sub_dir2</t>
@@ -157,7 +129,7 @@
     <t xml:space="preserve">Track2_2</t>
   </si>
   <si>
-    <t xml:space="preserve">test-hub/test2_2.Bigbed</t>
+    <t xml:space="preserve">test3.Bigbed</t>
   </si>
   <si>
     <t xml:space="preserve">t2.2</t>
@@ -176,7 +148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -221,12 +193,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -319,11 +285,11 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.14"/>
@@ -389,7 +355,7 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.79"/>
@@ -436,8 +402,8 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>